<commit_message>
SHIP-1 DPE changed harmonisation rule for kaffee and tee
</commit_message>
<xml_diff>
--- a/analyst/Franzi/rmonize/data_proc_elem/DPE_SHIP_FRANZI.xlsx
+++ b/analyst/Franzi/rmonize/data_proc_elem/DPE_SHIP_FRANZI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Franzi\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{0961438D-63D9-444F-B199-BB113C221031}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{6EEA2D0B-3386-40D0-87C5-20A8A737AFB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="320">
   <si>
     <t>index</t>
   </si>
@@ -887,9 +887,6 @@
   </si>
   <si>
     <t>only frequency</t>
-  </si>
-  <si>
-    <t>food_24 + food_25 + food_21</t>
   </si>
   <si>
     <t>food_8;food_9</t>
@@ -1030,6 +1027,15 @@
   </si>
   <si>
     <t>food_8;food_9;food_13;food_14;food_15;food_16</t>
+  </si>
+  <si>
+    <t>food_23 + food_24 + food_25 + food_21</t>
+  </si>
+  <si>
+    <t>schnwe; schnwt</t>
+  </si>
+  <si>
+    <t>schnwe + schnwt</t>
   </si>
 </sst>
 </file>
@@ -1460,8 +1466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="J93" sqref="J93"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="K90" sqref="K90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,7 +1475,7 @@
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
@@ -2116,13 +2122,13 @@
         <v>282</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G22" t="s">
         <v>287</v>
       </c>
       <c r="H22" t="s">
-        <v>289</v>
+        <v>317</v>
       </c>
       <c r="I22" t="s">
         <v>288</v>
@@ -2148,13 +2154,13 @@
         <v>282</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G23" t="s">
         <v>287</v>
       </c>
       <c r="H23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I23" t="s">
         <v>288</v>
@@ -2180,13 +2186,13 @@
         <v>282</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G24" t="s">
         <v>287</v>
       </c>
       <c r="H24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I24" t="s">
         <v>288</v>
@@ -2450,13 +2456,13 @@
         <v>282</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G33" t="s">
         <v>287</v>
       </c>
       <c r="H33" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I33" t="s">
         <v>288</v>
@@ -2511,13 +2517,13 @@
         <v>282</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G35" t="s">
         <v>287</v>
       </c>
       <c r="H35" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I35" t="s">
         <v>288</v>
@@ -2543,13 +2549,13 @@
         <v>282</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G36" t="s">
         <v>287</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I36" t="s">
         <v>288</v>
@@ -2581,7 +2587,7 @@
         <v>287</v>
       </c>
       <c r="H37" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I37" t="s">
         <v>288</v>
@@ -2758,7 +2764,7 @@
         <v>282</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G43" t="s">
         <v>276</v>
@@ -3199,13 +3205,13 @@
         <v>282</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G58" t="s">
         <v>287</v>
       </c>
       <c r="H58" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I58" t="s">
         <v>288</v>
@@ -3440,13 +3446,13 @@
         <v>282</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G66" t="s">
         <v>287</v>
       </c>
       <c r="H66" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I66" t="s">
         <v>288</v>
@@ -3472,13 +3478,13 @@
         <v>282</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G67" t="s">
         <v>287</v>
       </c>
       <c r="H67" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I67" t="s">
         <v>288</v>
@@ -4009,13 +4015,13 @@
         <v>282</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G85" t="s">
         <v>287</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I85" t="s">
         <v>288</v>
@@ -4137,13 +4143,13 @@
         <v>275</v>
       </c>
       <c r="G89" t="s">
-        <v>276</v>
+        <v>287</v>
       </c>
       <c r="H89" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J89" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K89" t="s">
         <v>281</v>
@@ -4166,13 +4172,13 @@
         <v>279</v>
       </c>
       <c r="G90" t="s">
-        <v>276</v>
+        <v>287</v>
       </c>
       <c r="H90" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J90" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K90" t="s">
         <v>281</v>
@@ -4282,7 +4288,7 @@
         <v>282</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G94" t="s">
         <v>276</v>
@@ -4291,10 +4297,10 @@
         <v>276</v>
       </c>
       <c r="I94" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J94" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K94" t="s">
         <v>278</v>
@@ -4314,17 +4320,17 @@
         <v>282</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G95" t="s">
         <v>287</v>
       </c>
       <c r="H95" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I95" s="7"/>
       <c r="J95" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K95" t="s">
         <v>281</v>
@@ -4373,16 +4379,16 @@
         <v>282</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G97" t="s">
         <v>287</v>
       </c>
       <c r="H97" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J97" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K97" t="s">
         <v>281</v>
@@ -4402,19 +4408,19 @@
         <v>282</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>256</v>
+        <v>318</v>
       </c>
       <c r="G98" t="s">
-        <v>256</v>
+        <v>287</v>
       </c>
       <c r="H98" t="s">
-        <v>256</v>
+        <v>319</v>
       </c>
       <c r="J98" s="2" t="s">
-        <v>256</v>
+        <v>277</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
     </row>
     <row r="99" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
SHIP-1 changed dietary assessment category in DPE
</commit_message>
<xml_diff>
--- a/analyst/Franzi/rmonize/data_proc_elem/DPE_SHIP_FRANZI.xlsx
+++ b/analyst/Franzi/rmonize/data_proc_elem/DPE_SHIP_FRANZI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Franzi\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{6EEA2D0B-3386-40D0-87C5-20A8A737AFB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{9200EB9F-7D9E-43D2-ADEC-108EB58821BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -875,9 +875,6 @@
   </si>
   <si>
     <t>paste</t>
-  </si>
-  <si>
-    <t>1 (FFQ)</t>
   </si>
   <si>
     <t>food_6 +  food_7</t>
@@ -1036,6 +1033,9 @@
   </si>
   <si>
     <t>schnwe + schnwt</t>
+  </si>
+  <si>
+    <t>0 (FPQ)</t>
   </si>
 </sst>
 </file>
@@ -1466,8 +1466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="K90" sqref="K90"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="I121" sqref="I121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,13 +1533,13 @@
         <v>253</v>
       </c>
       <c r="G2" t="s">
+        <v>286</v>
+      </c>
+      <c r="H2" t="s">
+        <v>285</v>
+      </c>
+      <c r="I2" t="s">
         <v>287</v>
-      </c>
-      <c r="H2" t="s">
-        <v>286</v>
-      </c>
-      <c r="I2" t="s">
-        <v>288</v>
       </c>
       <c r="J2" t="s">
         <v>254</v>
@@ -1565,13 +1565,13 @@
         <v>253</v>
       </c>
       <c r="G3" t="s">
+        <v>286</v>
+      </c>
+      <c r="H3" t="s">
+        <v>285</v>
+      </c>
+      <c r="I3" t="s">
         <v>287</v>
-      </c>
-      <c r="H3" t="s">
-        <v>286</v>
-      </c>
-      <c r="I3" t="s">
-        <v>288</v>
       </c>
       <c r="J3" t="s">
         <v>254</v>
@@ -1893,7 +1893,7 @@
         <v>276</v>
       </c>
       <c r="I14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>254</v>
@@ -2012,7 +2012,7 @@
         <v>276</v>
       </c>
       <c r="I18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>254</v>
@@ -2122,16 +2122,16 @@
         <v>282</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G22" t="s">
+        <v>286</v>
+      </c>
+      <c r="H22" t="s">
+        <v>316</v>
+      </c>
+      <c r="I22" t="s">
         <v>287</v>
-      </c>
-      <c r="H22" t="s">
-        <v>317</v>
-      </c>
-      <c r="I22" t="s">
-        <v>288</v>
       </c>
       <c r="J22" t="s">
         <v>254</v>
@@ -2154,16 +2154,16 @@
         <v>282</v>
       </c>
       <c r="F23" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G23" t="s">
+        <v>286</v>
+      </c>
+      <c r="H23" t="s">
         <v>313</v>
       </c>
-      <c r="G23" t="s">
+      <c r="I23" t="s">
         <v>287</v>
-      </c>
-      <c r="H23" t="s">
-        <v>314</v>
-      </c>
-      <c r="I23" t="s">
-        <v>288</v>
       </c>
       <c r="J23" t="s">
         <v>254</v>
@@ -2186,16 +2186,16 @@
         <v>282</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G24" t="s">
+        <v>286</v>
+      </c>
+      <c r="H24" t="s">
         <v>313</v>
       </c>
-      <c r="G24" t="s">
+      <c r="I24" t="s">
         <v>287</v>
-      </c>
-      <c r="H24" t="s">
-        <v>314</v>
-      </c>
-      <c r="I24" t="s">
-        <v>288</v>
       </c>
       <c r="J24" t="s">
         <v>254</v>
@@ -2285,7 +2285,7 @@
         <v>276</v>
       </c>
       <c r="I27" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J27" t="s">
         <v>254</v>
@@ -2346,7 +2346,7 @@
         <v>276</v>
       </c>
       <c r="I29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>254</v>
@@ -2456,16 +2456,16 @@
         <v>282</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G33" t="s">
+        <v>286</v>
+      </c>
+      <c r="H33" t="s">
+        <v>314</v>
+      </c>
+      <c r="I33" t="s">
         <v>287</v>
-      </c>
-      <c r="H33" t="s">
-        <v>315</v>
-      </c>
-      <c r="I33" t="s">
-        <v>288</v>
       </c>
       <c r="J33" t="s">
         <v>254</v>
@@ -2517,16 +2517,16 @@
         <v>282</v>
       </c>
       <c r="F35" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="G35" t="s">
+        <v>286</v>
+      </c>
+      <c r="H35" t="s">
         <v>289</v>
       </c>
-      <c r="G35" t="s">
+      <c r="I35" t="s">
         <v>287</v>
-      </c>
-      <c r="H35" t="s">
-        <v>290</v>
-      </c>
-      <c r="I35" t="s">
-        <v>288</v>
       </c>
       <c r="J35" t="s">
         <v>254</v>
@@ -2549,16 +2549,16 @@
         <v>282</v>
       </c>
       <c r="F36" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="G36" t="s">
+        <v>286</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="G36" t="s">
+      <c r="I36" t="s">
         <v>287</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="I36" t="s">
-        <v>288</v>
       </c>
       <c r="J36" t="s">
         <v>254</v>
@@ -2584,13 +2584,13 @@
         <v>262</v>
       </c>
       <c r="G37" t="s">
+        <v>286</v>
+      </c>
+      <c r="H37" t="s">
+        <v>292</v>
+      </c>
+      <c r="I37" t="s">
         <v>287</v>
-      </c>
-      <c r="H37" t="s">
-        <v>293</v>
-      </c>
-      <c r="I37" t="s">
-        <v>288</v>
       </c>
       <c r="J37" t="s">
         <v>254</v>
@@ -2622,7 +2622,7 @@
         <v>276</v>
       </c>
       <c r="I38" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J38" t="s">
         <v>254</v>
@@ -2654,7 +2654,7 @@
         <v>276</v>
       </c>
       <c r="I39" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J39" t="s">
         <v>254</v>
@@ -2764,7 +2764,7 @@
         <v>282</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G43" t="s">
         <v>276</v>
@@ -2773,7 +2773,7 @@
         <v>276</v>
       </c>
       <c r="I43" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J43" t="s">
         <v>254</v>
@@ -2979,7 +2979,7 @@
         <v>276</v>
       </c>
       <c r="I50" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J50" t="s">
         <v>254</v>
@@ -3205,16 +3205,16 @@
         <v>282</v>
       </c>
       <c r="F58" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="G58" t="s">
+        <v>286</v>
+      </c>
+      <c r="H58" t="s">
         <v>295</v>
       </c>
-      <c r="G58" t="s">
+      <c r="I58" t="s">
         <v>287</v>
-      </c>
-      <c r="H58" t="s">
-        <v>296</v>
-      </c>
-      <c r="I58" t="s">
-        <v>288</v>
       </c>
       <c r="J58" t="s">
         <v>254</v>
@@ -3304,7 +3304,7 @@
         <v>276</v>
       </c>
       <c r="I61" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J61" t="s">
         <v>254</v>
@@ -3394,7 +3394,7 @@
         <v>276</v>
       </c>
       <c r="I64" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J64" t="s">
         <v>254</v>
@@ -3446,16 +3446,16 @@
         <v>282</v>
       </c>
       <c r="F66" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G66" t="s">
+        <v>286</v>
+      </c>
+      <c r="H66" t="s">
         <v>297</v>
       </c>
-      <c r="G66" t="s">
+      <c r="I66" t="s">
         <v>287</v>
-      </c>
-      <c r="H66" t="s">
-        <v>298</v>
-      </c>
-      <c r="I66" t="s">
-        <v>288</v>
       </c>
       <c r="J66" t="s">
         <v>254</v>
@@ -3478,16 +3478,16 @@
         <v>282</v>
       </c>
       <c r="F67" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G67" t="s">
+        <v>286</v>
+      </c>
+      <c r="H67" t="s">
         <v>299</v>
       </c>
-      <c r="G67" t="s">
+      <c r="I67" t="s">
         <v>287</v>
-      </c>
-      <c r="H67" t="s">
-        <v>300</v>
-      </c>
-      <c r="I67" t="s">
-        <v>288</v>
       </c>
       <c r="J67" t="s">
         <v>254</v>
@@ -3519,7 +3519,7 @@
         <v>276</v>
       </c>
       <c r="I68" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J68" t="s">
         <v>254</v>
@@ -3551,7 +3551,7 @@
         <v>276</v>
       </c>
       <c r="I69" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J69" t="s">
         <v>254</v>
@@ -3670,7 +3670,7 @@
         <v>276</v>
       </c>
       <c r="I73" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J73" t="s">
         <v>254</v>
@@ -3934,7 +3934,7 @@
         <v>276</v>
       </c>
       <c r="I82" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J82" t="s">
         <v>254</v>
@@ -4015,16 +4015,16 @@
         <v>282</v>
       </c>
       <c r="F85" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="G85" t="s">
+        <v>286</v>
+      </c>
+      <c r="H85" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="G85" t="s">
+      <c r="I85" t="s">
         <v>287</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="I85" t="s">
-        <v>288</v>
       </c>
       <c r="J85" t="s">
         <v>254</v>
@@ -4056,7 +4056,7 @@
         <v>276</v>
       </c>
       <c r="I86" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J86" t="s">
         <v>254</v>
@@ -4088,7 +4088,7 @@
         <v>276</v>
       </c>
       <c r="I87" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J87" t="s">
         <v>254</v>
@@ -4143,13 +4143,13 @@
         <v>275</v>
       </c>
       <c r="G89" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H89" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J89" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K89" t="s">
         <v>281</v>
@@ -4172,13 +4172,13 @@
         <v>279</v>
       </c>
       <c r="G90" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H90" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J90" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K90" t="s">
         <v>281</v>
@@ -4265,7 +4265,7 @@
         <v>276</v>
       </c>
       <c r="I93" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J93" t="s">
         <v>254</v>
@@ -4288,7 +4288,7 @@
         <v>282</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G94" t="s">
         <v>276</v>
@@ -4297,10 +4297,10 @@
         <v>276</v>
       </c>
       <c r="I94" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J94" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K94" t="s">
         <v>278</v>
@@ -4320,17 +4320,17 @@
         <v>282</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G95" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H95" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I95" s="7"/>
       <c r="J95" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K95" t="s">
         <v>281</v>
@@ -4379,16 +4379,16 @@
         <v>282</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G97" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H97" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J97" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K97" t="s">
         <v>281</v>
@@ -4408,13 +4408,13 @@
         <v>282</v>
       </c>
       <c r="F98" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="G98" t="s">
+        <v>286</v>
+      </c>
+      <c r="H98" t="s">
         <v>318</v>
-      </c>
-      <c r="G98" t="s">
-        <v>287</v>
-      </c>
-      <c r="H98" t="s">
-        <v>319</v>
       </c>
       <c r="J98" s="2" t="s">
         <v>277</v>
@@ -5026,7 +5026,7 @@
         <v>276</v>
       </c>
       <c r="I119" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J119" t="s">
         <v>254</v>
@@ -5084,10 +5084,10 @@
         <v>284</v>
       </c>
       <c r="H121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I121" t="s">
-        <v>285</v>
+        <v>319</v>
       </c>
       <c r="J121" t="s">
         <v>277</v>

</xml_diff>

<commit_message>
SHIP-1 DPE: changes in the operation for wine, beer and spirits
</commit_message>
<xml_diff>
--- a/analyst/Franzi/rmonize/data_proc_elem/DPE_SHIP_FRANZI.xlsx
+++ b/analyst/Franzi/rmonize/data_proc_elem/DPE_SHIP_FRANZI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Franzi\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{9200EB9F-7D9E-43D2-ADEC-108EB58821BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{47DAE868-88A7-422A-B764-730A1F472EB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="321">
   <si>
     <t>index</t>
   </si>
@@ -781,9 +781,6 @@
     <t>integer</t>
   </si>
   <si>
-    <t>food_6; food_7</t>
-  </si>
-  <si>
     <t>partial</t>
   </si>
   <si>
@@ -806,9 +803,6 @@
   </si>
   <si>
     <t>food_21</t>
-  </si>
-  <si>
-    <t>food_13; food_15</t>
   </si>
   <si>
     <t>food_14</t>
@@ -971,12 +965,6 @@
   </si>
   <si>
     <t>bierwe;bierwt</t>
-  </si>
-  <si>
-    <t>weinwe + weinwt</t>
-  </si>
-  <si>
-    <t>bierwe + bierwt</t>
   </si>
   <si>
     <t>food_23;food_24;food_25;food_21</t>
@@ -1029,13 +1017,28 @@
     <t>food_23 + food_24 + food_25 + food_21</t>
   </si>
   <si>
-    <t>schnwe; schnwt</t>
-  </si>
-  <si>
-    <t>schnwe + schnwt</t>
-  </si>
-  <si>
     <t>0 (FPQ)</t>
+  </si>
+  <si>
+    <t>schnwe;schnwt</t>
+  </si>
+  <si>
+    <t>food_13;food_15</t>
+  </si>
+  <si>
+    <t>food_6;food_7</t>
+  </si>
+  <si>
+    <t>(weinwe + weinwt)/2</t>
+  </si>
+  <si>
+    <t>(bierwe + bierwt)/2</t>
+  </si>
+  <si>
+    <t>(schnwe + schnwt)/2</t>
+  </si>
+  <si>
+    <t>average intake from exemplary weekday and weekend</t>
   </si>
 </sst>
 </file>
@@ -1466,22 +1469,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="I121" sqref="I121"/>
+    <sheetView tabSelected="1" topLeftCell="B78" workbookViewId="0">
+      <selection activeCell="H100" sqref="H100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1516,7 +1519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1527,28 +1530,28 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G2" t="s">
+        <v>284</v>
+      </c>
+      <c r="H2" t="s">
+        <v>283</v>
+      </c>
+      <c r="I2" t="s">
+        <v>285</v>
+      </c>
+      <c r="J2" t="s">
         <v>253</v>
       </c>
-      <c r="G2" t="s">
-        <v>286</v>
-      </c>
-      <c r="H2" t="s">
-        <v>285</v>
-      </c>
-      <c r="I2" t="s">
-        <v>287</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>254</v>
       </c>
-      <c r="K2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1559,28 +1562,28 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G3" t="s">
+        <v>284</v>
+      </c>
+      <c r="H3" t="s">
+        <v>283</v>
+      </c>
+      <c r="I3" t="s">
+        <v>285</v>
+      </c>
+      <c r="J3" t="s">
         <v>253</v>
       </c>
-      <c r="G3" t="s">
-        <v>286</v>
-      </c>
-      <c r="H3" t="s">
-        <v>285</v>
-      </c>
-      <c r="I3" t="s">
-        <v>287</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>254</v>
       </c>
-      <c r="K3" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -1591,25 +1594,25 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -1620,25 +1623,25 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -1649,25 +1652,25 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>22</v>
       </c>
@@ -1678,25 +1681,25 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -1707,25 +1710,25 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>26</v>
       </c>
@@ -1736,25 +1739,25 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>28</v>
       </c>
@@ -1765,25 +1768,25 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>30</v>
       </c>
@@ -1794,25 +1797,25 @@
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>32</v>
       </c>
@@ -1823,25 +1826,25 @@
         <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>34</v>
       </c>
@@ -1852,25 +1855,25 @@
         <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>36</v>
       </c>
@@ -1881,28 +1884,28 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J14" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="K14" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>38</v>
       </c>
@@ -1913,25 +1916,25 @@
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>40</v>
       </c>
@@ -1942,25 +1945,25 @@
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>42</v>
       </c>
@@ -1971,25 +1974,25 @@
         <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>44</v>
       </c>
@@ -2000,28 +2003,28 @@
         <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G18" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H18" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I18" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J18" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="K18" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="K18" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>46</v>
       </c>
@@ -2032,25 +2035,25 @@
         <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>48</v>
       </c>
@@ -2061,25 +2064,25 @@
         <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>50</v>
       </c>
@@ -2090,25 +2093,25 @@
         <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>52</v>
       </c>
@@ -2119,28 +2122,28 @@
         <v>13</v>
       </c>
       <c r="E22" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="G22" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H22" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="I22" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J22" t="s">
+        <v>253</v>
+      </c>
+      <c r="K22" t="s">
         <v>254</v>
       </c>
-      <c r="K22" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>54</v>
       </c>
@@ -2151,28 +2154,28 @@
         <v>13</v>
       </c>
       <c r="E23" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="G23" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H23" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="I23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J23" t="s">
+        <v>253</v>
+      </c>
+      <c r="K23" t="s">
         <v>254</v>
       </c>
-      <c r="K23" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>56</v>
       </c>
@@ -2183,28 +2186,28 @@
         <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="G24" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H24" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="I24" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J24" t="s">
+        <v>253</v>
+      </c>
+      <c r="K24" t="s">
         <v>254</v>
       </c>
-      <c r="K24" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>58</v>
       </c>
@@ -2215,25 +2218,25 @@
         <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>60</v>
       </c>
@@ -2244,25 +2247,25 @@
         <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>62</v>
       </c>
@@ -2273,28 +2276,28 @@
         <v>13</v>
       </c>
       <c r="E27" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G27" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H27" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I27" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J27" t="s">
+        <v>253</v>
+      </c>
+      <c r="K27" t="s">
         <v>254</v>
       </c>
-      <c r="K27" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>64</v>
       </c>
@@ -2305,25 +2308,25 @@
         <v>13</v>
       </c>
       <c r="E28" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G28" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H28" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>66</v>
       </c>
@@ -2334,28 +2337,28 @@
         <v>13</v>
       </c>
       <c r="E29" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G29" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H29" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I29" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J29" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="K29" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>68</v>
       </c>
@@ -2366,25 +2369,25 @@
         <v>13</v>
       </c>
       <c r="E30" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>70</v>
       </c>
@@ -2395,25 +2398,25 @@
         <v>13</v>
       </c>
       <c r="E31" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>72</v>
       </c>
@@ -2424,25 +2427,25 @@
         <v>13</v>
       </c>
       <c r="E32" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>74</v>
       </c>
@@ -2453,28 +2456,28 @@
         <v>13</v>
       </c>
       <c r="E33" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="G33" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H33" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="I33" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J33" t="s">
+        <v>253</v>
+      </c>
+      <c r="K33" t="s">
         <v>254</v>
       </c>
-      <c r="K33" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>76</v>
       </c>
@@ -2485,25 +2488,25 @@
         <v>13</v>
       </c>
       <c r="E34" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>78</v>
       </c>
@@ -2514,28 +2517,28 @@
         <v>13</v>
       </c>
       <c r="E35" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G35" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H35" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I35" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J35" t="s">
+        <v>253</v>
+      </c>
+      <c r="K35" t="s">
         <v>254</v>
       </c>
-      <c r="K35" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>80</v>
       </c>
@@ -2546,28 +2549,28 @@
         <v>13</v>
       </c>
       <c r="E36" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G36" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I36" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J36" t="s">
+        <v>253</v>
+      </c>
+      <c r="K36" t="s">
         <v>254</v>
       </c>
-      <c r="K36" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>82</v>
       </c>
@@ -2578,28 +2581,28 @@
         <v>13</v>
       </c>
       <c r="E37" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>262</v>
+        <v>315</v>
       </c>
       <c r="G37" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H37" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I37" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J37" t="s">
+        <v>253</v>
+      </c>
+      <c r="K37" t="s">
         <v>254</v>
       </c>
-      <c r="K37" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>84</v>
       </c>
@@ -2610,28 +2613,28 @@
         <v>13</v>
       </c>
       <c r="E38" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G38" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H38" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I38" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J38" t="s">
+        <v>253</v>
+      </c>
+      <c r="K38" t="s">
         <v>254</v>
       </c>
-      <c r="K38" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>86</v>
       </c>
@@ -2642,28 +2645,28 @@
         <v>13</v>
       </c>
       <c r="E39" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G39" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H39" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I39" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J39" t="s">
+        <v>253</v>
+      </c>
+      <c r="K39" t="s">
         <v>254</v>
       </c>
-      <c r="K39" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>88</v>
       </c>
@@ -2674,25 +2677,25 @@
         <v>13</v>
       </c>
       <c r="E40" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G40" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H40" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J40" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K40" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>90</v>
       </c>
@@ -2703,25 +2706,25 @@
         <v>13</v>
       </c>
       <c r="E41" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G41" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H41" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>92</v>
       </c>
@@ -2732,25 +2735,25 @@
         <v>13</v>
       </c>
       <c r="E42" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G42" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H42" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>94</v>
       </c>
@@ -2761,28 +2764,28 @@
         <v>13</v>
       </c>
       <c r="E43" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G43" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H43" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I43" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J43" t="s">
+        <v>253</v>
+      </c>
+      <c r="K43" t="s">
         <v>254</v>
       </c>
-      <c r="K43" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>96</v>
       </c>
@@ -2793,25 +2796,25 @@
         <v>13</v>
       </c>
       <c r="E44" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G44" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H44" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>98</v>
       </c>
@@ -2822,25 +2825,25 @@
         <v>13</v>
       </c>
       <c r="E45" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G45" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H45" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>100</v>
       </c>
@@ -2851,25 +2854,25 @@
         <v>13</v>
       </c>
       <c r="E46" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G46" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H46" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>102</v>
       </c>
@@ -2880,25 +2883,25 @@
         <v>13</v>
       </c>
       <c r="E47" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G47" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H47" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>104</v>
       </c>
@@ -2909,25 +2912,25 @@
         <v>13</v>
       </c>
       <c r="E48" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G48" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H48" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>106</v>
       </c>
@@ -2938,25 +2941,25 @@
         <v>13</v>
       </c>
       <c r="E49" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G49" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H49" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>108</v>
       </c>
@@ -2967,28 +2970,28 @@
         <v>13</v>
       </c>
       <c r="E50" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G50" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H50" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I50" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J50" t="s">
+        <v>253</v>
+      </c>
+      <c r="K50" t="s">
         <v>254</v>
       </c>
-      <c r="K50" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>110</v>
       </c>
@@ -2999,25 +3002,25 @@
         <v>13</v>
       </c>
       <c r="E51" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G51" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H51" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>112</v>
       </c>
@@ -3028,25 +3031,25 @@
         <v>13</v>
       </c>
       <c r="E52" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G52" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H52" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>114</v>
       </c>
@@ -3057,25 +3060,25 @@
         <v>13</v>
       </c>
       <c r="E53" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G53" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H53" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>116</v>
       </c>
@@ -3086,25 +3089,25 @@
         <v>13</v>
       </c>
       <c r="E54" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G54" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H54" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>118</v>
       </c>
@@ -3115,25 +3118,25 @@
         <v>13</v>
       </c>
       <c r="E55" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G55" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H55" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>120</v>
       </c>
@@ -3144,25 +3147,25 @@
         <v>13</v>
       </c>
       <c r="E56" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G56" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H56" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>122</v>
       </c>
@@ -3173,25 +3176,25 @@
         <v>13</v>
       </c>
       <c r="E57" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G57" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H57" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>124</v>
       </c>
@@ -3202,28 +3205,28 @@
         <v>13</v>
       </c>
       <c r="E58" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G58" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H58" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I58" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J58" t="s">
+        <v>253</v>
+      </c>
+      <c r="K58" t="s">
         <v>254</v>
       </c>
-      <c r="K58" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>126</v>
       </c>
@@ -3234,25 +3237,25 @@
         <v>13</v>
       </c>
       <c r="E59" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G59" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H59" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>128</v>
       </c>
@@ -3263,25 +3266,25 @@
         <v>13</v>
       </c>
       <c r="E60" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G60" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H60" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>130</v>
       </c>
@@ -3292,28 +3295,28 @@
         <v>13</v>
       </c>
       <c r="E61" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G61" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H61" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I61" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J61" t="s">
+        <v>253</v>
+      </c>
+      <c r="K61" t="s">
         <v>254</v>
       </c>
-      <c r="K61" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>132</v>
       </c>
@@ -3324,25 +3327,25 @@
         <v>13</v>
       </c>
       <c r="E62" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G62" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H62" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>134</v>
       </c>
@@ -3353,25 +3356,25 @@
         <v>13</v>
       </c>
       <c r="E63" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G63" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H63" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>136</v>
       </c>
@@ -3382,28 +3385,28 @@
         <v>13</v>
       </c>
       <c r="E64" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G64" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H64" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I64" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J64" t="s">
+        <v>253</v>
+      </c>
+      <c r="K64" t="s">
         <v>254</v>
       </c>
-      <c r="K64" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>138</v>
       </c>
@@ -3414,25 +3417,25 @@
         <v>13</v>
       </c>
       <c r="E65" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G65" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H65" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>140</v>
       </c>
@@ -3443,28 +3446,28 @@
         <v>13</v>
       </c>
       <c r="E66" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G66" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H66" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I66" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J66" t="s">
+        <v>253</v>
+      </c>
+      <c r="K66" t="s">
         <v>254</v>
       </c>
-      <c r="K66" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>142</v>
       </c>
@@ -3475,28 +3478,28 @@
         <v>13</v>
       </c>
       <c r="E67" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G67" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H67" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I67" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J67" t="s">
+        <v>253</v>
+      </c>
+      <c r="K67" t="s">
         <v>254</v>
       </c>
-      <c r="K67" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>144</v>
       </c>
@@ -3507,28 +3510,28 @@
         <v>13</v>
       </c>
       <c r="E68" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G68" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H68" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I68" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J68" t="s">
+        <v>253</v>
+      </c>
+      <c r="K68" t="s">
         <v>254</v>
       </c>
-      <c r="K68" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>146</v>
       </c>
@@ -3539,28 +3542,28 @@
         <v>13</v>
       </c>
       <c r="E69" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G69" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H69" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I69" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J69" t="s">
+        <v>253</v>
+      </c>
+      <c r="K69" t="s">
         <v>254</v>
       </c>
-      <c r="K69" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>148</v>
       </c>
@@ -3571,25 +3574,25 @@
         <v>13</v>
       </c>
       <c r="E70" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G70" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H70" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>150</v>
       </c>
@@ -3600,25 +3603,25 @@
         <v>13</v>
       </c>
       <c r="E71" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G71" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H71" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>152</v>
       </c>
@@ -3629,25 +3632,25 @@
         <v>13</v>
       </c>
       <c r="E72" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G72" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H72" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>154</v>
       </c>
@@ -3658,28 +3661,28 @@
         <v>13</v>
       </c>
       <c r="E73" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G73" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H73" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I73" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J73" t="s">
+        <v>253</v>
+      </c>
+      <c r="K73" t="s">
         <v>254</v>
       </c>
-      <c r="K73" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>156</v>
       </c>
@@ -3690,25 +3693,25 @@
         <v>13</v>
       </c>
       <c r="E74" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G74" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H74" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>158</v>
       </c>
@@ -3719,25 +3722,25 @@
         <v>13</v>
       </c>
       <c r="E75" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G75" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H75" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>160</v>
       </c>
@@ -3748,25 +3751,25 @@
         <v>13</v>
       </c>
       <c r="E76" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G76" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H76" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>162</v>
       </c>
@@ -3777,25 +3780,25 @@
         <v>13</v>
       </c>
       <c r="E77" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G77" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H77" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>164</v>
       </c>
@@ -3806,25 +3809,25 @@
         <v>13</v>
       </c>
       <c r="E78" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G78" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H78" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>166</v>
       </c>
@@ -3835,25 +3838,25 @@
         <v>13</v>
       </c>
       <c r="E79" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G79" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H79" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J79" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>168</v>
       </c>
@@ -3864,25 +3867,25 @@
         <v>13</v>
       </c>
       <c r="E80" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G80" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H80" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J80" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>170</v>
       </c>
@@ -3893,25 +3896,25 @@
         <v>13</v>
       </c>
       <c r="E81" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G81" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H81" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J81" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>172</v>
       </c>
@@ -3922,28 +3925,28 @@
         <v>13</v>
       </c>
       <c r="E82" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G82" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H82" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I82" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J82" t="s">
+        <v>253</v>
+      </c>
+      <c r="K82" t="s">
         <v>254</v>
       </c>
-      <c r="K82" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>174</v>
       </c>
@@ -3954,25 +3957,25 @@
         <v>13</v>
       </c>
       <c r="E83" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G83" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H83" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J83" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>176</v>
       </c>
@@ -3983,25 +3986,25 @@
         <v>13</v>
       </c>
       <c r="E84" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J84" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
         <v>178</v>
       </c>
@@ -4012,28 +4015,28 @@
         <v>13</v>
       </c>
       <c r="E85" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G85" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I85" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J85" t="s">
+        <v>253</v>
+      </c>
+      <c r="K85" t="s">
         <v>254</v>
       </c>
-      <c r="K85" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>180</v>
       </c>
@@ -4044,28 +4047,28 @@
         <v>13</v>
       </c>
       <c r="E86" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G86" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H86" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I86" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J86" t="s">
+        <v>253</v>
+      </c>
+      <c r="K86" t="s">
         <v>254</v>
       </c>
-      <c r="K86" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>182</v>
       </c>
@@ -4076,28 +4079,28 @@
         <v>13</v>
       </c>
       <c r="E87" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F87" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="G87" t="s">
         <v>274</v>
       </c>
-      <c r="G87" t="s">
-        <v>276</v>
-      </c>
       <c r="H87" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I87" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J87" t="s">
+        <v>253</v>
+      </c>
+      <c r="K87" t="s">
         <v>254</v>
       </c>
-      <c r="K87" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>184</v>
       </c>
@@ -4108,25 +4111,25 @@
         <v>13</v>
       </c>
       <c r="E88" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G88" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H88" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J88" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>186</v>
       </c>
@@ -4137,25 +4140,25 @@
         <v>13</v>
       </c>
       <c r="E89" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G89" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H89" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J89" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="K89" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>188</v>
       </c>
@@ -4166,25 +4169,25 @@
         <v>13</v>
       </c>
       <c r="E90" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F90" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="G90" t="s">
+        <v>284</v>
+      </c>
+      <c r="H90" t="s">
+        <v>302</v>
+      </c>
+      <c r="J90" t="s">
+        <v>300</v>
+      </c>
+      <c r="K90" t="s">
         <v>279</v>
       </c>
-      <c r="G90" t="s">
-        <v>286</v>
-      </c>
-      <c r="H90" t="s">
-        <v>304</v>
-      </c>
-      <c r="J90" t="s">
-        <v>302</v>
-      </c>
-      <c r="K90" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>190</v>
       </c>
@@ -4195,25 +4198,25 @@
         <v>13</v>
       </c>
       <c r="E91" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G91" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H91" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J91" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>192</v>
       </c>
@@ -4224,25 +4227,25 @@
         <v>13</v>
       </c>
       <c r="E92" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G92" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H92" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J92" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>194</v>
       </c>
@@ -4253,28 +4256,28 @@
         <v>13</v>
       </c>
       <c r="E93" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G93" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H93" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I93" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J93" t="s">
+        <v>253</v>
+      </c>
+      <c r="K93" t="s">
         <v>254</v>
       </c>
-      <c r="K93" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="94" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>196</v>
       </c>
@@ -4285,28 +4288,28 @@
         <v>13</v>
       </c>
       <c r="E94" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G94" t="s">
+        <v>274</v>
+      </c>
+      <c r="H94" t="s">
+        <v>274</v>
+      </c>
+      <c r="I94" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="J94" t="s">
+        <v>300</v>
+      </c>
+      <c r="K94" t="s">
         <v>276</v>
       </c>
-      <c r="H94" t="s">
-        <v>276</v>
-      </c>
-      <c r="I94" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="J94" t="s">
-        <v>302</v>
-      </c>
-      <c r="K94" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>198</v>
       </c>
@@ -4317,26 +4320,28 @@
         <v>13</v>
       </c>
       <c r="E95" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G95" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H95" t="s">
-        <v>309</v>
-      </c>
-      <c r="I95" s="7"/>
+        <v>317</v>
+      </c>
+      <c r="I95" s="7" t="s">
+        <v>320</v>
+      </c>
       <c r="J95" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="K95" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>200</v>
       </c>
@@ -4347,25 +4352,25 @@
         <v>13</v>
       </c>
       <c r="E96" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G96" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H96" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>202</v>
       </c>
@@ -4376,25 +4381,28 @@
         <v>13</v>
       </c>
       <c r="E97" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G97" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H97" t="s">
-        <v>310</v>
+        <v>318</v>
+      </c>
+      <c r="I97" s="7" t="s">
+        <v>320</v>
       </c>
       <c r="J97" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="K97" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>204</v>
       </c>
@@ -4405,25 +4413,28 @@
         <v>13</v>
       </c>
       <c r="E98" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G98" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H98" t="s">
-        <v>318</v>
+        <v>319</v>
+      </c>
+      <c r="I98" s="7" t="s">
+        <v>320</v>
       </c>
       <c r="J98" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>206</v>
       </c>
@@ -4434,25 +4445,25 @@
         <v>13</v>
       </c>
       <c r="E99" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G99" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H99" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J99" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>208</v>
       </c>
@@ -4463,25 +4474,25 @@
         <v>13</v>
       </c>
       <c r="E100" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G100" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H100" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J100" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>210</v>
       </c>
@@ -4492,25 +4503,25 @@
         <v>13</v>
       </c>
       <c r="E101" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G101" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H101" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J101" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>212</v>
       </c>
@@ -4521,25 +4532,25 @@
         <v>13</v>
       </c>
       <c r="E102" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G102" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H102" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J102" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>214</v>
       </c>
@@ -4550,25 +4561,25 @@
         <v>13</v>
       </c>
       <c r="E103" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G103" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H103" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J103" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K103" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="104" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>216</v>
       </c>
@@ -4579,25 +4590,25 @@
         <v>13</v>
       </c>
       <c r="E104" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G104" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H104" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J104" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K104" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>218</v>
       </c>
@@ -4608,25 +4619,25 @@
         <v>13</v>
       </c>
       <c r="E105" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G105" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H105" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J105" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K105" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="106" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
         <v>220</v>
       </c>
@@ -4637,25 +4648,25 @@
         <v>13</v>
       </c>
       <c r="E106" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G106" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H106" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J106" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K106" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="107" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>222</v>
       </c>
@@ -4666,25 +4677,25 @@
         <v>13</v>
       </c>
       <c r="E107" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G107" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H107" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J107" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K107" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="108" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="108" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
         <v>224</v>
       </c>
@@ -4695,25 +4706,25 @@
         <v>13</v>
       </c>
       <c r="E108" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G108" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H108" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J108" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="109" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B109" t="s">
         <v>226</v>
       </c>
@@ -4724,25 +4735,25 @@
         <v>13</v>
       </c>
       <c r="E109" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G109" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H109" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J109" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K109" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="110" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
         <v>228</v>
       </c>
@@ -4753,25 +4764,25 @@
         <v>13</v>
       </c>
       <c r="E110" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G110" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H110" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J110" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K110" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B111" t="s">
         <v>230</v>
       </c>
@@ -4782,25 +4793,25 @@
         <v>13</v>
       </c>
       <c r="E111" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G111" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H111" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J111" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="112" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="112" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
         <v>232</v>
       </c>
@@ -4811,25 +4822,25 @@
         <v>13</v>
       </c>
       <c r="E112" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G112" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H112" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J112" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="113" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="113" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B113" t="s">
         <v>234</v>
       </c>
@@ -4840,25 +4851,25 @@
         <v>13</v>
       </c>
       <c r="E113" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G113" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H113" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J113" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K113" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="114" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="114" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
         <v>236</v>
       </c>
@@ -4869,25 +4880,25 @@
         <v>13</v>
       </c>
       <c r="E114" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G114" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H114" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J114" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K114" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="115" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="115" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>238</v>
       </c>
@@ -4898,25 +4909,25 @@
         <v>13</v>
       </c>
       <c r="E115" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G115" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H115" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J115" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K115" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="116" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="116" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
         <v>240</v>
       </c>
@@ -4927,25 +4938,25 @@
         <v>13</v>
       </c>
       <c r="E116" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J116" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K116" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="117" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="117" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
         <v>242</v>
       </c>
@@ -4956,25 +4967,25 @@
         <v>13</v>
       </c>
       <c r="E117" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G117" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H117" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J117" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K117" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="118" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="118" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
         <v>244</v>
       </c>
@@ -4985,25 +4996,25 @@
         <v>13</v>
       </c>
       <c r="E118" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G118" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H118" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J118" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K118" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="119" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="119" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
         <v>246</v>
       </c>
@@ -5014,28 +5025,28 @@
         <v>13</v>
       </c>
       <c r="E119" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G119" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H119" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I119" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J119" t="s">
+        <v>253</v>
+      </c>
+      <c r="K119" t="s">
         <v>254</v>
       </c>
-      <c r="K119" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="120" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>248</v>
       </c>
@@ -5046,25 +5057,25 @@
         <v>13</v>
       </c>
       <c r="E120" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G120" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H120" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J120" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K120" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="121" spans="2:11" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="121" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B121" t="s">
         <v>250</v>
       </c>
@@ -5075,28 +5086,28 @@
         <v>252</v>
       </c>
       <c r="E121" t="s">
+        <v>280</v>
+      </c>
+      <c r="F121" t="s">
+        <v>281</v>
+      </c>
+      <c r="G121" t="s">
         <v>282</v>
-      </c>
-      <c r="F121" t="s">
-        <v>283</v>
-      </c>
-      <c r="G121" t="s">
-        <v>284</v>
       </c>
       <c r="H121">
         <v>0</v>
       </c>
       <c r="I121" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="J121" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="K121" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="122" spans="2:11" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="122" spans="2:11" x14ac:dyDescent="0.3">
       <c r="F122" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SHIP-5 DD and DPE files incl their comparables in P1 and P2 style before first discussion meeting
</commit_message>
<xml_diff>
--- a/analyst/Franzi/rmonize/data_proc_elem/DPE_SHIP_FRANZI.xlsx
+++ b/analyst/Franzi/rmonize/data_proc_elem/DPE_SHIP_FRANZI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Franzi\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\analyst\Franzi\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{47DAE868-88A7-422A-B764-730A1F472EB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4AC372-D8D5-4CDA-B946-3CCFEE5D7800}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -863,9 +863,6 @@
   </si>
   <si>
     <t>SHIP_P1</t>
-  </si>
-  <si>
-    <t>_BLANK_</t>
   </si>
   <si>
     <t>paste</t>
@@ -1039,6 +1036,9 @@
   </si>
   <si>
     <t>average intake from exemplary weekday and weekend</t>
+  </si>
+  <si>
+    <t>__BLANK__</t>
   </si>
 </sst>
 </file>
@@ -1469,22 +1469,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B78" workbookViewId="0">
-      <selection activeCell="H100" sqref="H100"/>
+    <sheetView tabSelected="1" topLeftCell="B106" workbookViewId="0">
+      <selection activeCell="F121" sqref="F121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1533,16 +1533,16 @@
         <v>280</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G2" t="s">
+        <v>283</v>
+      </c>
+      <c r="H2" t="s">
+        <v>282</v>
+      </c>
+      <c r="I2" t="s">
         <v>284</v>
-      </c>
-      <c r="H2" t="s">
-        <v>283</v>
-      </c>
-      <c r="I2" t="s">
-        <v>285</v>
       </c>
       <c r="J2" t="s">
         <v>253</v>
@@ -1551,7 +1551,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1565,16 +1565,16 @@
         <v>280</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G3" t="s">
+        <v>283</v>
+      </c>
+      <c r="H3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I3" t="s">
         <v>284</v>
-      </c>
-      <c r="H3" t="s">
-        <v>283</v>
-      </c>
-      <c r="I3" t="s">
-        <v>285</v>
       </c>
       <c r="J3" t="s">
         <v>253</v>
@@ -1583,7 +1583,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>22</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>26</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>28</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>30</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>32</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>34</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>36</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>274</v>
       </c>
       <c r="I14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>253</v>
@@ -1905,7 +1905,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>38</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>40</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>42</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>44</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>274</v>
       </c>
       <c r="I18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>253</v>
@@ -2024,7 +2024,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>46</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>48</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>50</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>52</v>
       </c>
@@ -2125,16 +2125,16 @@
         <v>280</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G22" t="s">
+        <v>283</v>
+      </c>
+      <c r="H22" t="s">
+        <v>311</v>
+      </c>
+      <c r="I22" t="s">
         <v>284</v>
-      </c>
-      <c r="H22" t="s">
-        <v>312</v>
-      </c>
-      <c r="I22" t="s">
-        <v>285</v>
       </c>
       <c r="J22" t="s">
         <v>253</v>
@@ -2143,7 +2143,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>54</v>
       </c>
@@ -2157,16 +2157,16 @@
         <v>280</v>
       </c>
       <c r="F23" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="G23" t="s">
+        <v>283</v>
+      </c>
+      <c r="H23" t="s">
         <v>308</v>
       </c>
-      <c r="G23" t="s">
+      <c r="I23" t="s">
         <v>284</v>
-      </c>
-      <c r="H23" t="s">
-        <v>309</v>
-      </c>
-      <c r="I23" t="s">
-        <v>285</v>
       </c>
       <c r="J23" t="s">
         <v>253</v>
@@ -2175,7 +2175,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>56</v>
       </c>
@@ -2189,16 +2189,16 @@
         <v>280</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="G24" t="s">
+        <v>283</v>
+      </c>
+      <c r="H24" t="s">
         <v>308</v>
       </c>
-      <c r="G24" t="s">
+      <c r="I24" t="s">
         <v>284</v>
-      </c>
-      <c r="H24" t="s">
-        <v>309</v>
-      </c>
-      <c r="I24" t="s">
-        <v>285</v>
       </c>
       <c r="J24" t="s">
         <v>253</v>
@@ -2207,7 +2207,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>58</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>60</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>62</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>274</v>
       </c>
       <c r="I27" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J27" t="s">
         <v>253</v>
@@ -2297,7 +2297,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>64</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>66</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>274</v>
       </c>
       <c r="I29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>253</v>
@@ -2358,7 +2358,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>68</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>70</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>72</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>74</v>
       </c>
@@ -2459,16 +2459,16 @@
         <v>280</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G33" t="s">
+        <v>283</v>
+      </c>
+      <c r="H33" t="s">
+        <v>309</v>
+      </c>
+      <c r="I33" t="s">
         <v>284</v>
-      </c>
-      <c r="H33" t="s">
-        <v>310</v>
-      </c>
-      <c r="I33" t="s">
-        <v>285</v>
       </c>
       <c r="J33" t="s">
         <v>253</v>
@@ -2477,7 +2477,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>76</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>78</v>
       </c>
@@ -2520,16 +2520,16 @@
         <v>280</v>
       </c>
       <c r="F35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="G35" t="s">
+        <v>283</v>
+      </c>
+      <c r="H35" t="s">
         <v>286</v>
       </c>
-      <c r="G35" t="s">
+      <c r="I35" t="s">
         <v>284</v>
-      </c>
-      <c r="H35" t="s">
-        <v>287</v>
-      </c>
-      <c r="I35" t="s">
-        <v>285</v>
       </c>
       <c r="J35" t="s">
         <v>253</v>
@@ -2538,7 +2538,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>80</v>
       </c>
@@ -2552,16 +2552,16 @@
         <v>280</v>
       </c>
       <c r="F36" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G36" t="s">
+        <v>283</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="G36" t="s">
+      <c r="I36" t="s">
         <v>284</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="I36" t="s">
-        <v>285</v>
       </c>
       <c r="J36" t="s">
         <v>253</v>
@@ -2570,7 +2570,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>82</v>
       </c>
@@ -2584,16 +2584,16 @@
         <v>280</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G37" t="s">
+        <v>283</v>
+      </c>
+      <c r="H37" t="s">
+        <v>289</v>
+      </c>
+      <c r="I37" t="s">
         <v>284</v>
-      </c>
-      <c r="H37" t="s">
-        <v>290</v>
-      </c>
-      <c r="I37" t="s">
-        <v>285</v>
       </c>
       <c r="J37" t="s">
         <v>253</v>
@@ -2602,7 +2602,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>84</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>274</v>
       </c>
       <c r="I38" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J38" t="s">
         <v>253</v>
@@ -2634,7 +2634,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>86</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>274</v>
       </c>
       <c r="I39" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J39" t="s">
         <v>253</v>
@@ -2666,7 +2666,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>88</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>90</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>92</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>94</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>280</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G43" t="s">
         <v>274</v>
@@ -2776,7 +2776,7 @@
         <v>274</v>
       </c>
       <c r="I43" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J43" t="s">
         <v>253</v>
@@ -2785,7 +2785,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>96</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>98</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>100</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>102</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>104</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>106</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>108</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>274</v>
       </c>
       <c r="I50" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J50" t="s">
         <v>253</v>
@@ -2991,7 +2991,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>110</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>112</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>114</v>
       </c>
@@ -3078,7 +3078,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>116</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>118</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>120</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>122</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>124</v>
       </c>
@@ -3208,16 +3208,16 @@
         <v>280</v>
       </c>
       <c r="F58" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="G58" t="s">
+        <v>283</v>
+      </c>
+      <c r="H58" t="s">
         <v>292</v>
       </c>
-      <c r="G58" t="s">
+      <c r="I58" t="s">
         <v>284</v>
-      </c>
-      <c r="H58" t="s">
-        <v>293</v>
-      </c>
-      <c r="I58" t="s">
-        <v>285</v>
       </c>
       <c r="J58" t="s">
         <v>253</v>
@@ -3226,7 +3226,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>126</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>128</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>130</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>274</v>
       </c>
       <c r="I61" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J61" t="s">
         <v>253</v>
@@ -3316,7 +3316,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>132</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>134</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>136</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>274</v>
       </c>
       <c r="I64" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J64" t="s">
         <v>253</v>
@@ -3406,7 +3406,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>138</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>140</v>
       </c>
@@ -3449,16 +3449,16 @@
         <v>280</v>
       </c>
       <c r="F66" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="G66" t="s">
+        <v>283</v>
+      </c>
+      <c r="H66" t="s">
         <v>294</v>
       </c>
-      <c r="G66" t="s">
+      <c r="I66" t="s">
         <v>284</v>
-      </c>
-      <c r="H66" t="s">
-        <v>295</v>
-      </c>
-      <c r="I66" t="s">
-        <v>285</v>
       </c>
       <c r="J66" t="s">
         <v>253</v>
@@ -3467,7 +3467,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>142</v>
       </c>
@@ -3481,16 +3481,16 @@
         <v>280</v>
       </c>
       <c r="F67" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G67" t="s">
+        <v>283</v>
+      </c>
+      <c r="H67" t="s">
         <v>296</v>
       </c>
-      <c r="G67" t="s">
+      <c r="I67" t="s">
         <v>284</v>
-      </c>
-      <c r="H67" t="s">
-        <v>297</v>
-      </c>
-      <c r="I67" t="s">
-        <v>285</v>
       </c>
       <c r="J67" t="s">
         <v>253</v>
@@ -3499,7 +3499,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>144</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>274</v>
       </c>
       <c r="I68" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J68" t="s">
         <v>253</v>
@@ -3531,7 +3531,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>146</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>274</v>
       </c>
       <c r="I69" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J69" t="s">
         <v>253</v>
@@ -3563,7 +3563,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>148</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>150</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>152</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>154</v>
       </c>
@@ -3673,7 +3673,7 @@
         <v>274</v>
       </c>
       <c r="I73" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J73" t="s">
         <v>253</v>
@@ -3682,7 +3682,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>156</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>158</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>160</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>162</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>164</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>166</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>168</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>170</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>172</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>274</v>
       </c>
       <c r="I82" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J82" t="s">
         <v>253</v>
@@ -3946,7 +3946,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>174</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>176</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>178</v>
       </c>
@@ -4018,16 +4018,16 @@
         <v>280</v>
       </c>
       <c r="F85" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="G85" t="s">
+        <v>283</v>
+      </c>
+      <c r="H85" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="G85" t="s">
+      <c r="I85" t="s">
         <v>284</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="I85" t="s">
-        <v>285</v>
       </c>
       <c r="J85" t="s">
         <v>253</v>
@@ -4036,7 +4036,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>180</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>274</v>
       </c>
       <c r="I86" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J86" t="s">
         <v>253</v>
@@ -4068,7 +4068,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>182</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>274</v>
       </c>
       <c r="I87" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J87" t="s">
         <v>253</v>
@@ -4100,7 +4100,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>184</v>
       </c>
@@ -4129,7 +4129,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>186</v>
       </c>
@@ -4146,19 +4146,19 @@
         <v>273</v>
       </c>
       <c r="G89" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H89" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J89" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K89" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>188</v>
       </c>
@@ -4175,19 +4175,19 @@
         <v>277</v>
       </c>
       <c r="G90" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H90" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J90" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K90" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>190</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>192</v>
       </c>
@@ -4245,7 +4245,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>194</v>
       </c>
@@ -4268,7 +4268,7 @@
         <v>274</v>
       </c>
       <c r="I93" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J93" t="s">
         <v>253</v>
@@ -4277,7 +4277,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="94" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>196</v>
       </c>
@@ -4291,7 +4291,7 @@
         <v>280</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G94" t="s">
         <v>274</v>
@@ -4300,16 +4300,16 @@
         <v>274</v>
       </c>
       <c r="I94" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J94" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K94" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>198</v>
       </c>
@@ -4323,25 +4323,25 @@
         <v>280</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G95" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H95" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I95" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J95" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K95" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>200</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>202</v>
       </c>
@@ -4384,25 +4384,25 @@
         <v>280</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G97" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H97" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I97" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J97" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K97" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>204</v>
       </c>
@@ -4416,16 +4416,16 @@
         <v>280</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G98" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H98" t="s">
+        <v>318</v>
+      </c>
+      <c r="I98" s="7" t="s">
         <v>319</v>
-      </c>
-      <c r="I98" s="7" t="s">
-        <v>320</v>
       </c>
       <c r="J98" s="2" t="s">
         <v>275</v>
@@ -4434,7 +4434,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>206</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>208</v>
       </c>
@@ -4492,7 +4492,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>210</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>212</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>214</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>216</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>218</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>220</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>222</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="108" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>224</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>226</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>228</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>230</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="112" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>232</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="113" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>234</v>
       </c>
@@ -4869,7 +4869,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="114" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>236</v>
       </c>
@@ -4898,7 +4898,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="115" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>238</v>
       </c>
@@ -4927,7 +4927,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="116" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>240</v>
       </c>
@@ -4956,7 +4956,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="117" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>242</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="118" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>244</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="119" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>246</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>274</v>
       </c>
       <c r="I119" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J119" t="s">
         <v>253</v>
@@ -5046,7 +5046,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="120" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>248</v>
       </c>
@@ -5075,7 +5075,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="121" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>250</v>
       </c>
@@ -5089,16 +5089,16 @@
         <v>280</v>
       </c>
       <c r="F121" t="s">
+        <v>320</v>
+      </c>
+      <c r="G121" t="s">
         <v>281</v>
-      </c>
-      <c r="G121" t="s">
-        <v>282</v>
       </c>
       <c r="H121">
         <v>0</v>
       </c>
       <c r="I121" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J121" t="s">
         <v>275</v>
@@ -5107,7 +5107,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="122" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F122" s="2"/>
     </row>
   </sheetData>

</xml_diff>